<commit_message>
Adding convolutional layer success
</commit_message>
<xml_diff>
--- a/Keras Model Log.xlsx
+++ b/Keras Model Log.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabernbaum/Documents/GitHub/SoloProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559B218C-9BA8-A34F-9A47-A0C60A4DF5C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7C346A-1E5E-454D-80C3-DFA0403E320D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{214E882B-C77D-3449-B769-D95BD346DE52}"/>
+    <workbookView xWindow="38940" yWindow="4760" windowWidth="28040" windowHeight="16440" xr2:uid="{214E882B-C77D-3449-B769-D95BD346DE52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Model Name</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t xml:space="preserve">Mel, Dense full 128, Flatten, Dense sigmoid, </t>
+  </si>
+  <si>
+    <t>First 2D Convolutional Attempt on Single Tagged Clips</t>
+  </si>
+  <si>
+    <t>Added a 2D Conv and Leaky Relu</t>
+  </si>
+  <si>
+    <t>Mel, conv2d, leakyrelu, flatten, dense</t>
+  </si>
+  <si>
+    <t>True Negatives</t>
+  </si>
+  <si>
+    <t>Actual Accuracy</t>
   </si>
 </sst>
 </file>
@@ -121,10 +136,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,15 +455,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701F9ED3-E3FA-E84F-86E6-0EF8BEE30077}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
@@ -455,7 +472,7 @@
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +492,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -486,8 +503,11 @@
       <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -507,16 +527,56 @@
         <v>0.73</v>
       </c>
       <c r="G2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H2">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="J2">
-        <v>46</v>
+        <v>31</v>
+      </c>
+      <c r="K2" s="3">
+        <f>(G2+J2)/SUM(G2:J2)</f>
+        <v>0.67567567567567566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>3.6</v>
+      </c>
+      <c r="F3">
+        <v>0.77</v>
+      </c>
+      <c r="G3">
+        <v>48</v>
+      </c>
+      <c r="H3">
+        <v>11</v>
+      </c>
+      <c r="I3">
+        <v>14</v>
+      </c>
+      <c r="J3">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3">
+        <f>(G3+J3)/SUM(G3:J3)</f>
+        <v>0.77477477477477474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued work, RMS, validation
</commit_message>
<xml_diff>
--- a/Keras Model Log.xlsx
+++ b/Keras Model Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabernbaum/Documents/GitHub/SoloProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7C346A-1E5E-454D-80C3-DFA0403E320D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29943DDD-5E10-5542-906B-0F20457E99F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38940" yWindow="4760" windowWidth="28040" windowHeight="16440" xr2:uid="{214E882B-C77D-3449-B769-D95BD346DE52}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{214E882B-C77D-3449-B769-D95BD346DE52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Model Name</t>
   </si>
@@ -85,6 +85,66 @@
   </si>
   <si>
     <t>Actual Accuracy</t>
+  </si>
+  <si>
+    <t>Same layers, reduced spectrogram resolution</t>
+  </si>
+  <si>
+    <t>2D Conv reduced melspec</t>
+  </si>
+  <si>
+    <t>Second 2D Convolutional Attempt on Single Tagged Clips</t>
+  </si>
+  <si>
+    <t>Repeat of 1st</t>
+  </si>
+  <si>
+    <t>appears to be overfitting</t>
+  </si>
+  <si>
+    <t>Same as before but, n_dft=256, n_hop=128</t>
+  </si>
+  <si>
+    <t>Repeat but reduce spec resolution</t>
+  </si>
+  <si>
+    <t>next:</t>
+  </si>
+  <si>
+    <t>validation set</t>
+  </si>
+  <si>
+    <t>another conv layer</t>
+  </si>
+  <si>
+    <t>runs very slow</t>
+  </si>
+  <si>
+    <t>Redcued mel spec</t>
+  </si>
+  <si>
+    <t>with val</t>
+  </si>
+  <si>
+    <t>Repeat with validation set (shouldn’t make a difference)</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>One pool</t>
+  </si>
+  <si>
+    <t>Adding a single pool layer</t>
+  </si>
+  <si>
+    <t>Double original</t>
+  </si>
+  <si>
+    <t>original 3 layers x 2</t>
+  </si>
+  <si>
+    <t>Mel, conv2d, leakyrelu, pool, conv2d, leakyrelu, flatten, dense</t>
   </si>
 </sst>
 </file>
@@ -455,15 +515,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701F9ED3-E3FA-E84F-86E6-0EF8BEE30077}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
@@ -472,7 +532,7 @@
     <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -543,7 +603,7 @@
         <v>0.67567567567567566</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -577,6 +637,167 @@
       <c r="K3" s="3">
         <f>(G3+J3)/SUM(G3:J3)</f>
         <v>0.77477477477477474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="G4">
+        <v>47</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>64</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K7" si="0">(G4+J4)/SUM(G4:J4)</f>
+        <v>0.42342342342342343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>3.48</v>
+      </c>
+      <c r="F5">
+        <v>0.78</v>
+      </c>
+      <c r="G5">
+        <v>57</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>30</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.78378378378378377</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>3.97</v>
+      </c>
+      <c r="F7">
+        <v>0.75</v>
+      </c>
+      <c r="G7">
+        <v>32</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>19</v>
+      </c>
+      <c r="J7">
+        <v>33</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.7303370786516854</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
successful models! corrected eval rounding bug
</commit_message>
<xml_diff>
--- a/Keras Model Log.xlsx
+++ b/Keras Model Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabernbaum/Documents/GitHub/SoloProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC09833C-9002-D747-9BB3-7E69AD48453F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B0435C-9943-B74E-A0EA-46F34026996D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" xr2:uid="{214E882B-C77D-3449-B769-D95BD346DE52}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
   <si>
     <t>Model Name</t>
   </si>
@@ -199,6 +199,50 @@
   </si>
   <si>
     <t>still all answers are cough</t>
+  </si>
+  <si>
+    <t>opals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model = keras.Sequential()
+input_shape = (1, 220500)
+sr = 22050  # Sampling rate of the audio
+model.add(Melspectrogram(n_dft=512, n_hop=256, input_shape=input_shape,
+                         padding='same', sr=sr, n_mels=128,
+                         fmin=0.0, fmax=sr/2, power_melgram=1.0,
+                         return_decibel_melgram=False, trainable_fb=False,
+                         trainable_kernel=False,
+                         name='trainable_stft'))
+model.add(keras.layers.Conv2D(128, [7,11], strides=[2,2], padding = 'SAME'))
+model.add(keras.layers.LeakyReLU(alpha=0.1))
+model.add(keras.layers.MaxPool2D(pool_size=(2,2), padding='SAME'))
+model.add(keras.layers.Conv2D(128, [7,11], strides=[2,2], padding = 'SAME'))
+model.add(keras.layers.LeakyReLU(alpha=0.1))
+# model.add(keras.layers.Dropout(0.5))
+model.add(keras.layers.Flatten())
+model.add(keras.layers.Dense(1, activation='sigmoid'))
+</t>
+  </si>
+  <si>
+    <t>CORRECTED CONFUSION MATRIX AT THIS POINT</t>
+  </si>
+  <si>
+    <t>pringle</t>
+  </si>
+  <si>
+    <t>same as above but with early stopping</t>
+  </si>
+  <si>
+    <t>same as above with a 0.5 dropout at the end</t>
+  </si>
+  <si>
+    <t>same as above bu 0.2 dropout at end</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>same as before but 3nd conv kernel size 64, no dropiut</t>
   </si>
 </sst>
 </file>
@@ -250,11 +294,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701F9ED3-E3FA-E84F-86E6-0EF8BEE30077}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" ref="K4:K18" si="0">(G4+J4)/SUM(G4:J4)</f>
+        <f t="shared" ref="K4:K22" si="0">(G4+J4)/SUM(G4:J4)</f>
         <v>0.42342342342342343</v>
       </c>
     </row>
@@ -1137,8 +1182,133 @@
         <v>55</v>
       </c>
     </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19">
+        <v>1.33</v>
+      </c>
+      <c r="F19">
+        <v>0.81</v>
+      </c>
+      <c r="G19">
+        <v>46</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>16</v>
+      </c>
+      <c r="J19">
+        <v>26</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.8089887640449438</v>
+      </c>
+      <c r="L19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20">
+        <v>0.53</v>
+      </c>
+      <c r="F20">
+        <v>0.78</v>
+      </c>
+      <c r="G20">
+        <v>45</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>18</v>
+      </c>
+      <c r="J20">
+        <v>24</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.7752808988764045</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21">
+        <v>4.45</v>
+      </c>
+      <c r="F21">
+        <v>0.68</v>
+      </c>
+      <c r="G21">
+        <v>33</v>
+      </c>
+      <c r="H21">
+        <v>14</v>
+      </c>
+      <c r="I21">
+        <v>14</v>
+      </c>
+      <c r="J21">
+        <v>28</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="0"/>
+        <v>0.6853932584269663</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F22">
+        <v>0.84</v>
+      </c>
+      <c r="G22">
+        <v>44</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>11</v>
+      </c>
+      <c r="J22">
+        <v>31</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="0"/>
+        <v>0.84269662921348309</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K18">
+  <conditionalFormatting sqref="K2:K22">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1150,7 +1320,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F18">
+  <conditionalFormatting sqref="F2:F22">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1162,7 +1332,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E18">
+  <conditionalFormatting sqref="E2:E22">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>